<commit_message>
[NaV] Grobe Änderungen im Terminplan
</commit_message>
<xml_diff>
--- a/Termine.xlsx
+++ b/Termine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\HS-AMR-Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DBCAF9D-B823-48A1-B687-F36759026359}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9493A07-504C-4101-B0CA-588146B3D775}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2CFC9008-4A6F-4317-8C54-829ACB1CB81D}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>Datum</t>
   </si>
@@ -183,6 +183,45 @@
   </si>
   <si>
     <t>Bedienung fertig</t>
+  </si>
+  <si>
+    <t>Weitere Termine:</t>
+  </si>
+  <si>
+    <t>2 Wochen vor 2. Verteidigung</t>
+  </si>
+  <si>
+    <t>2 Wochen vor Abgabe der Doku.</t>
+  </si>
+  <si>
+    <t>[ALL] Testphase beginnen --&gt; Codes müssen fertig sein</t>
+  </si>
+  <si>
+    <t>[ALL] Abgabe Dokumentation</t>
+  </si>
+  <si>
+    <t>3 Tage vor 1. Verteidigung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[NAV] Lokalisierung durch Radodometrie + Fusion + Posenschätzung fertig </t>
+  </si>
+  <si>
+    <t>[NAV] Parklückendedektion Basisfunktionsumfang fertig</t>
+  </si>
+  <si>
+    <t>[NAV] Bewertung Parklücken + Verbessrungsmanöver fertig</t>
+  </si>
+  <si>
+    <t>17.11.19 bis 23:59</t>
+  </si>
+  <si>
+    <t>10.11.19 bis 23:59</t>
+  </si>
+  <si>
+    <t>24.11.19 bis  23:59</t>
+  </si>
+  <si>
+    <t>[ALL]: Testphase abgeschlossen + [GUI] Zustandsautomaten Entwurf fertig</t>
   </si>
 </sst>
 </file>
@@ -362,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -435,6 +474,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -755,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC9D805F-F956-40D3-8865-13C1FA595852}">
-  <dimension ref="B1:J24"/>
+  <dimension ref="B1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:G14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1127,10 +1172,64 @@
       <c r="E21" s="5"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="E23" s="5"/>
+      <c r="E23" s="39" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.35">
       <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="E25" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="E26" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="E27" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="E29" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="E30" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="E31" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>